<commit_message>
fixed preferences based on location preferences
</commit_message>
<xml_diff>
--- a/input/Longitudinal Ambulatory Block Preferences(1-14).xlsx
+++ b/input/Longitudinal Ambulatory Block Preferences(1-14).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lodhar/Projects/clerkshipscheduler/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A5A71E-AC1A-4246-A913-F0316FE708F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBB0F6C5-5FA1-CA46-A1BA-0549CB923DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -682,7 +682,7 @@
   <dimension ref="A1:L15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -783,9 +783,6 @@
       <c r="G3" t="s">
         <v>21</v>
       </c>
-      <c r="H3" t="s">
-        <v>15</v>
-      </c>
       <c r="I3" t="s">
         <v>22</v>
       </c>
@@ -821,9 +818,6 @@
       <c r="G4" t="s">
         <v>28</v>
       </c>
-      <c r="H4" t="s">
-        <v>15</v>
-      </c>
       <c r="I4" t="s">
         <v>22</v>
       </c>
@@ -892,9 +886,6 @@
       <c r="F6" s="1"/>
       <c r="G6" t="s">
         <v>38</v>
-      </c>
-      <c r="H6" t="s">
-        <v>15</v>
       </c>
       <c r="I6" t="s">
         <v>39</v>

</xml_diff>